<commit_message>
Kernprogramm nun voll Funktionsfähig
</commit_message>
<xml_diff>
--- a/doc/CookieClicker-Zeitplanung.xlsx
+++ b/doc/CookieClicker-Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenox\Desktop\cookie-clicker-2.0\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9DB535B0-3736-4B44-BDB0-A5695EC70B05}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{7FD0A50B-6C22-44B5-8E6A-17FC754AC3F8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -2116,22 +2116,22 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
       <selection activeCell="Q21" sqref="Q21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.625" style="5" customWidth="1"/>
-    <col min="2" max="2" width="31.875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="5.25" style="5" customWidth="1"/>
-    <col min="4" max="4" width="5.25" style="13" customWidth="1"/>
-    <col min="5" max="6" width="5.25" style="5" customWidth="1"/>
-    <col min="7" max="62" width="2.25" style="5" customWidth="1"/>
+    <col min="1" max="1" width="3.59765625" style="5" customWidth="1"/>
+    <col min="2" max="2" width="31.8984375" style="5" customWidth="1"/>
+    <col min="3" max="3" width="5.19921875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="5.19921875" style="13" customWidth="1"/>
+    <col min="5" max="6" width="5.19921875" style="5" customWidth="1"/>
+    <col min="7" max="62" width="2.19921875" style="5" customWidth="1"/>
     <col min="63" max="16384" width="12.5" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" ht="25.2" x14ac:dyDescent="0.3">
       <c r="A1" s="24" t="s">
         <v>16</v>
       </c>
@@ -2165,7 +2165,7 @@
       <c r="AC1" s="4"/>
       <c r="AD1" s="4"/>
     </row>
-    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:62" ht="5.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="6"/>
       <c r="B2" s="6"/>
       <c r="C2" s="6"/>
@@ -2229,7 +2229,7 @@
       <c r="BI2" s="6"/>
       <c r="BJ2" s="6"/>
     </row>
-    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6"/>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -2295,7 +2295,7 @@
       <c r="BI3" s="6"/>
       <c r="BJ3" s="6"/>
     </row>
-    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:62" ht="6.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="6"/>
       <c r="C4" s="6"/>
@@ -2359,7 +2359,7 @@
       <c r="BI4" s="6"/>
       <c r="BJ4" s="6"/>
     </row>
-    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2425,7 +2425,7 @@
       <c r="BI5" s="6"/>
       <c r="BJ5" s="6"/>
     </row>
-    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:62" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="7"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2433,7 +2433,7 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:62" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="9"/>
       <c r="B7" s="27"/>
       <c r="C7" s="90" t="s">
@@ -2519,7 +2519,7 @@
       <c r="BI7" s="91"/>
       <c r="BJ7" s="94"/>
     </row>
-    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:62" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="10" t="s">
         <v>0</v>
       </c>
@@ -2705,7 +2705,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="30">
         <v>10</v>
       </c>
@@ -2779,7 +2779,7 @@
       <c r="BI9" s="74"/>
       <c r="BJ9" s="78"/>
     </row>
-    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="12">
         <v>101</v>
       </c>
@@ -2855,7 +2855,7 @@
       <c r="BI10" s="57"/>
       <c r="BJ10" s="58"/>
     </row>
-    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11">
         <v>102</v>
       </c>
@@ -2938,7 +2938,7 @@
       <c r="BI11" s="57"/>
       <c r="BJ11" s="58"/>
     </row>
-    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11">
         <v>103</v>
       </c>
@@ -3015,7 +3015,7 @@
       <c r="BI12" s="57"/>
       <c r="BJ12" s="58"/>
     </row>
-    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11">
         <v>104</v>
       </c>
@@ -3089,7 +3089,7 @@
       <c r="BI13" s="66"/>
       <c r="BJ13" s="67"/>
     </row>
-    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30">
         <v>20</v>
       </c>
@@ -3163,7 +3163,7 @@
       <c r="BI14" s="74"/>
       <c r="BJ14" s="78"/>
     </row>
-    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="12">
         <v>201</v>
       </c>
@@ -3242,7 +3242,7 @@
       <c r="BI15" s="57"/>
       <c r="BJ15" s="58"/>
     </row>
-    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="12">
         <v>202</v>
       </c>
@@ -3319,7 +3319,7 @@
       <c r="BI16" s="57"/>
       <c r="BJ16" s="58"/>
     </row>
-    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="12">
         <v>203</v>
       </c>
@@ -3388,7 +3388,7 @@
       <c r="BI17" s="57"/>
       <c r="BJ17" s="58"/>
     </row>
-    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="30">
         <v>30</v>
       </c>
@@ -3462,7 +3462,7 @@
       <c r="BI18" s="74"/>
       <c r="BJ18" s="78"/>
     </row>
-    <row r="19" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="12">
         <v>301</v>
       </c>
@@ -3541,7 +3541,7 @@
       <c r="BI19" s="57"/>
       <c r="BJ19" s="58"/>
     </row>
-    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="12">
         <v>302</v>
       </c>
@@ -3620,7 +3620,7 @@
       <c r="BI20" s="57"/>
       <c r="BJ20" s="58"/>
     </row>
-    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="12">
         <v>303</v>
       </c>
@@ -3703,7 +3703,7 @@
       <c r="BI21" s="57"/>
       <c r="BJ21" s="58"/>
     </row>
-    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="12">
         <v>304</v>
       </c>
@@ -3780,7 +3780,7 @@
       <c r="BI22" s="57"/>
       <c r="BJ22" s="58"/>
     </row>
-    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="12">
         <v>305</v>
       </c>
@@ -3857,7 +3857,7 @@
       <c r="BI23" s="57"/>
       <c r="BJ23" s="58"/>
     </row>
-    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="12">
         <v>306</v>
       </c>
@@ -3932,7 +3932,7 @@
       <c r="BI24" s="57"/>
       <c r="BJ24" s="58"/>
     </row>
-    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="12">
         <v>307</v>
       </c>
@@ -4007,7 +4007,7 @@
       <c r="BI25" s="57"/>
       <c r="BJ25" s="58"/>
     </row>
-    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="12">
         <v>308</v>
       </c>
@@ -4082,7 +4082,7 @@
       <c r="BI26" s="57"/>
       <c r="BJ26" s="58"/>
     </row>
-    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="12">
         <v>309</v>
       </c>
@@ -4157,7 +4157,7 @@
       <c r="BI27" s="57"/>
       <c r="BJ27" s="58"/>
     </row>
-    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="12">
         <v>310</v>
       </c>
@@ -4232,7 +4232,7 @@
       <c r="BI28" s="57"/>
       <c r="BJ28" s="58"/>
     </row>
-    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="12">
         <v>311</v>
       </c>
@@ -4307,7 +4307,7 @@
       <c r="BI29" s="57"/>
       <c r="BJ29" s="58"/>
     </row>
-    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="12">
         <v>312</v>
       </c>
@@ -4376,7 +4376,7 @@
       <c r="BI30" s="57"/>
       <c r="BJ30" s="58"/>
     </row>
-    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="30">
         <v>40</v>
       </c>
@@ -4450,7 +4450,7 @@
       <c r="BI31" s="74"/>
       <c r="BJ31" s="78"/>
     </row>
-    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="12">
         <v>401</v>
       </c>
@@ -4523,7 +4523,7 @@
       <c r="BI32" s="57"/>
       <c r="BJ32" s="58"/>
     </row>
-    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="12">
         <v>402</v>
       </c>
@@ -4596,7 +4596,7 @@
       <c r="BI33" s="57"/>
       <c r="BJ33" s="58"/>
     </row>
-    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="12">
         <v>403</v>
       </c>
@@ -4669,7 +4669,7 @@
       <c r="BI34" s="57"/>
       <c r="BJ34" s="58"/>
     </row>
-    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="12">
         <v>404</v>
       </c>
@@ -4738,7 +4738,7 @@
       <c r="BI35" s="57"/>
       <c r="BJ35" s="58"/>
     </row>
-    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="30">
         <v>50</v>
       </c>
@@ -4812,7 +4812,7 @@
       <c r="BI36" s="74"/>
       <c r="BJ36" s="78"/>
     </row>
-    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="12">
         <v>501</v>
       </c>
@@ -4886,7 +4886,7 @@
       <c r="BI37" s="57"/>
       <c r="BJ37" s="58"/>
     </row>
-    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A38" s="12">
         <v>502</v>
       </c>
@@ -4955,7 +4955,7 @@
       <c r="BI38" s="57"/>
       <c r="BJ38" s="58"/>
     </row>
-    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="30">
         <v>60</v>
       </c>
@@ -5029,7 +5029,7 @@
       <c r="BI39" s="74"/>
       <c r="BJ39" s="78"/>
     </row>
-    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="12">
         <v>601</v>
       </c>
@@ -5102,7 +5102,7 @@
       <c r="BI40" s="57"/>
       <c r="BJ40" s="58"/>
     </row>
-    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="12">
         <v>602</v>
       </c>
@@ -5175,7 +5175,7 @@
       <c r="BI41" s="57"/>
       <c r="BJ41" s="58"/>
     </row>
-    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:62" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="12">
         <v>603</v>
       </c>
@@ -5244,7 +5244,7 @@
       <c r="BI42" s="57"/>
       <c r="BJ42" s="58"/>
     </row>
-    <row r="43" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:62" ht="17.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A43" s="35"/>
       <c r="B43" s="36" t="s">
         <v>6</v>
@@ -5519,17 +5519,17 @@
       <selection activeCell="O29" sqref="O29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="13.09765625" style="1" customWidth="1"/>
     <col min="2" max="2" width="12.5" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.5" style="1" customWidth="1"/>
-    <col min="4" max="4" width="9.25" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.19921875" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:6" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="15.6" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="1:6" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="97" t="s">
         <v>13</v>
       </c>
@@ -5541,7 +5541,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="95" t="str">
         <f>Zeitplanung!B9</f>
         <v>Administration, Planung</v>
@@ -5558,7 +5558,7 @@
       <c r="E3" s="82"/>
       <c r="F3" s="81"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="95" t="str">
         <f>Zeitplanung!B14</f>
         <v>Analyse &amp; Design</v>
@@ -5575,7 +5575,7 @@
       <c r="E4" s="82"/>
       <c r="F4" s="81"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="95" t="str">
         <f>Zeitplanung!B18</f>
         <v>Implementation</v>
@@ -5592,7 +5592,7 @@
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="95" t="str">
         <f>Zeitplanung!B31</f>
         <v>Testen</v>
@@ -5608,7 +5608,7 @@
       </c>
       <c r="F6" s="81"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="95" t="str">
         <f>Zeitplanung!B36</f>
         <v>Diverses</v>
@@ -5624,7 +5624,7 @@
       </c>
       <c r="F7" s="81"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="16.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="95" t="str">
         <f>Zeitplanung!B39</f>
         <v>Abschluss</v>
@@ -5640,7 +5640,7 @@
       </c>
       <c r="F8" s="81"/>
     </row>
-    <row r="9" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.2"/>
+    <row r="9" spans="1:6" ht="15.6" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="7">
     <mergeCell ref="A7:B7"/>

</xml_diff>

<commit_message>
general improvements + bug fixes
</commit_message>
<xml_diff>
--- a/doc/CookieClicker-Zeitplanung.xlsx
+++ b/doc/CookieClicker-Zeitplanung.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenox\Desktop\cookie-clicker-2.0\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E3DDA6B6-1502-4653-97F7-187791763CA0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3ED7EB98-2962-4E9A-A9A4-F8151D77468D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1609,7 +1609,7 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>39.5</c:v>
+                  <c:v>50.5</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2116,8 +2116,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="X26" sqref="X26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="Y29" sqref="Y29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>39.5</v>
+        <v>50.5</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3962,7 +3962,7 @@
       </c>
       <c r="D25" s="83">
         <f t="shared" si="0"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E25" s="50">
         <v>2</v>
@@ -3990,7 +3990,7 @@
         <v>7</v>
       </c>
       <c r="X25" s="63">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Y25" s="63"/>
       <c r="Z25" s="57"/>
@@ -4122,7 +4122,7 @@
       </c>
       <c r="D27" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E27" s="50">
         <v>2</v>
@@ -4145,8 +4145,12 @@
       <c r="U27" s="59"/>
       <c r="V27" s="60"/>
       <c r="W27" s="56"/>
-      <c r="X27" s="56"/>
-      <c r="Y27" s="56"/>
+      <c r="X27" s="56">
+        <v>2</v>
+      </c>
+      <c r="Y27" s="56">
+        <v>4</v>
+      </c>
       <c r="Z27" s="57"/>
       <c r="AA27" s="58"/>
       <c r="AB27" s="59"/>
@@ -4197,7 +4201,7 @@
       </c>
       <c r="D28" s="83">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E28" s="50">
         <v>3</v>
@@ -4221,7 +4225,9 @@
       <c r="V28" s="60"/>
       <c r="W28" s="56"/>
       <c r="X28" s="56"/>
-      <c r="Y28" s="56"/>
+      <c r="Y28" s="56">
+        <v>4</v>
+      </c>
       <c r="Z28" s="57"/>
       <c r="AA28" s="58"/>
       <c r="AB28" s="59"/>
@@ -5283,7 +5289,7 @@
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>49.5</v>
+        <v>60.5</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5357,11 +5363,11 @@
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="Y43" s="39">
         <f t="shared" si="3"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Z43" s="39">
         <f t="shared" si="3"/>
@@ -5615,7 +5621,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>39.5</v>
+        <v>50.5</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>

</xml_diff>

<commit_message>
Saving improved & minor improvements
</commit_message>
<xml_diff>
--- a/doc/CookieClicker-Zeitplanung.xlsx
+++ b/doc/CookieClicker-Zeitplanung.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenox\Desktop\cookie-clicker-2.0\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3ED7EB98-2962-4E9A-A9A4-F8151D77468D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5A96E987-0E1D-45E1-945A-FC60DB91F11D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="597" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8985" tabRatio="597" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Zeitplanung" sheetId="1" r:id="rId1"/>
@@ -1541,7 +1541,7 @@
                   <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>-0.5</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>3</c:v>
@@ -1609,16 +1609,16 @@
                   <c:v>5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.5</c:v>
+                  <c:v>51</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1717,7 +1717,7 @@
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="0.75000000000000333" l="0.70000000000000062" r="0.70000000000000062" t="0.75000000000000333" header="0.30000000000000032" footer="0.30000000000000032"/>
-    <c:pageSetup/>
+    <c:pageSetup orientation="landscape"/>
   </c:printSettings>
 </c:chartSpace>
 </file>
@@ -1726,16 +1726,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>916078</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>33617</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>154078</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>201707</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>459442</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>69476</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>403412</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>134471</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2116,8 +2116,8 @@
   </sheetPr>
   <dimension ref="A1:BJ43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="Y29" sqref="Y29"/>
+    <sheetView showGridLines="0" topLeftCell="A13" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="AY40" sqref="AY40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -3403,7 +3403,7 @@
       </c>
       <c r="D18" s="42">
         <f>SUM(D19:D30)</f>
-        <v>50.5</v>
+        <v>51</v>
       </c>
       <c r="E18" s="32"/>
       <c r="F18" s="31"/>
@@ -3658,9 +3658,7 @@
       <c r="P21" s="63">
         <v>1</v>
       </c>
-      <c r="Q21" s="87">
-        <v>0</v>
-      </c>
+      <c r="Q21" s="87"/>
       <c r="R21" s="56"/>
       <c r="S21" s="57"/>
       <c r="T21" s="58"/>
@@ -3828,9 +3826,7 @@
       <c r="T23" s="58"/>
       <c r="U23" s="59"/>
       <c r="V23" s="60"/>
-      <c r="W23" s="87">
-        <v>0</v>
-      </c>
+      <c r="W23" s="87"/>
       <c r="X23" s="61"/>
       <c r="Y23" s="56"/>
       <c r="Z23" s="57"/>
@@ -3907,9 +3903,7 @@
       <c r="T24" s="58"/>
       <c r="U24" s="59"/>
       <c r="V24" s="60"/>
-      <c r="W24" s="63">
-        <v>0</v>
-      </c>
+      <c r="W24" s="63"/>
       <c r="X24" s="56"/>
       <c r="Y24" s="56"/>
       <c r="Z24" s="57"/>
@@ -4043,7 +4037,7 @@
       </c>
       <c r="D26" s="83">
         <f t="shared" si="0"/>
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E26" s="50">
         <v>2</v>
@@ -4066,11 +4060,9 @@
       <c r="U26" s="59"/>
       <c r="V26" s="60"/>
       <c r="W26" s="63">
-        <v>0.5</v>
-      </c>
-      <c r="X26" s="63">
-        <v>0</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="X26" s="63"/>
       <c r="Y26" s="63"/>
       <c r="Z26" s="57"/>
       <c r="AA26" s="58"/>
@@ -4423,7 +4415,7 @@
       </c>
       <c r="D31" s="42">
         <f>SUM(D32:D35)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E31" s="32"/>
       <c r="F31" s="31"/>
@@ -4642,7 +4634,7 @@
       </c>
       <c r="D34" s="83">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E34" s="50"/>
       <c r="F34" s="51"/>
@@ -4683,8 +4675,12 @@
       <c r="AO34" s="58"/>
       <c r="AP34" s="59"/>
       <c r="AQ34" s="60"/>
-      <c r="AR34" s="63"/>
-      <c r="AS34" s="63"/>
+      <c r="AR34" s="63">
+        <v>4</v>
+      </c>
+      <c r="AS34" s="63">
+        <v>4</v>
+      </c>
       <c r="AT34" s="55"/>
       <c r="AU34" s="57"/>
       <c r="AV34" s="58"/>
@@ -4781,7 +4777,7 @@
       </c>
       <c r="C36" s="41">
         <f>SUM(C37:C38)</f>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D36" s="42">
         <f>SUM(D37:D38)</f>
@@ -4854,8 +4850,7 @@
         <v>27</v>
       </c>
       <c r="C37" s="49">
-        <f>-W26</f>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D37" s="83">
         <f>SUM(G37:BJ37)</f>
@@ -5002,7 +4997,7 @@
       </c>
       <c r="D39" s="42">
         <f>SUM(D40:D42)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E39" s="32"/>
       <c r="F39" s="31"/>
@@ -5075,7 +5070,7 @@
       </c>
       <c r="D40" s="83">
         <f>SUM(G40:BJ40)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E40" s="50"/>
       <c r="F40" s="51"/>
@@ -5116,8 +5111,12 @@
       <c r="AO40" s="58"/>
       <c r="AP40" s="53"/>
       <c r="AQ40" s="54"/>
-      <c r="AR40" s="55"/>
-      <c r="AS40" s="63"/>
+      <c r="AR40" s="55">
+        <v>4</v>
+      </c>
+      <c r="AS40" s="63">
+        <v>2</v>
+      </c>
       <c r="AT40" s="55"/>
       <c r="AU40" s="57"/>
       <c r="AV40" s="58"/>
@@ -5148,7 +5147,7 @@
       </c>
       <c r="D41" s="83">
         <f t="shared" ref="D41:D42" si="2">SUM(G41:BJ41)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E41" s="50"/>
       <c r="F41" s="51"/>
@@ -5190,7 +5189,9 @@
       <c r="AP41" s="59"/>
       <c r="AQ41" s="60"/>
       <c r="AR41" s="55"/>
-      <c r="AS41" s="63"/>
+      <c r="AS41" s="63">
+        <v>2</v>
+      </c>
       <c r="AT41" s="55"/>
       <c r="AU41" s="57"/>
       <c r="AV41" s="58"/>
@@ -5285,11 +5286,11 @@
       </c>
       <c r="C43" s="37">
         <f>C39+C36+C31+C18+C14+C9</f>
-        <v>65.5</v>
+        <v>66</v>
       </c>
       <c r="D43" s="37">
         <f>D39+D36+D31+D18+D14+D9</f>
-        <v>60.5</v>
+        <v>77</v>
       </c>
       <c r="E43" s="37"/>
       <c r="F43" s="38"/>
@@ -5359,7 +5360,7 @@
       </c>
       <c r="W43" s="39">
         <f t="shared" si="3"/>
-        <v>7.5</v>
+        <v>8</v>
       </c>
       <c r="X43" s="39">
         <f t="shared" si="3"/>
@@ -5443,11 +5444,11 @@
       </c>
       <c r="AR43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AS43" s="39">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AT43" s="39">
         <f t="shared" si="4"/>
@@ -5549,8 +5550,8 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="O29" sqref="O29"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -5621,7 +5622,7 @@
       </c>
       <c r="D5" s="80">
         <f>Zeitplanung!D18</f>
-        <v>50.5</v>
+        <v>51</v>
       </c>
       <c r="E5" s="82"/>
       <c r="F5" s="81"/>
@@ -5638,7 +5639,7 @@
       </c>
       <c r="D6" s="80">
         <f>Zeitplanung!D31</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F6" s="81"/>
     </row>
@@ -5650,7 +5651,7 @@
       <c r="B7" s="96"/>
       <c r="C7" s="80">
         <f>Zeitplanung!C36</f>
-        <v>-0.5</v>
+        <v>0</v>
       </c>
       <c r="D7" s="80">
         <f>Zeitplanung!D36</f>
@@ -5670,7 +5671,7 @@
       </c>
       <c r="D8" s="80">
         <f>Zeitplanung!D39</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="F8" s="81"/>
     </row>
@@ -5686,7 +5687,7 @@
     <mergeCell ref="A6:B6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="56" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" scale="95" orientation="landscape" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>